<commit_message>
2025-07-08 Added Kanji Images for n5
</commit_message>
<xml_diff>
--- a/public/docs/kanji_n5.xlsx
+++ b/public/docs/kanji_n5.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Kanji</t>
   </si>
@@ -33,100 +33,145 @@
     <t>にち / ひ</t>
   </si>
   <si>
+    <t>いち</t>
+  </si>
+  <si>
+    <t>one</t>
+  </si>
+  <si>
+    <t>くに</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>ひと</t>
+  </si>
+  <si>
+    <t>person</t>
+  </si>
+  <si>
+    <t>とし</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>おおきい</t>
+  </si>
+  <si>
+    <t>big</t>
+  </si>
+  <si>
+    <t>じゅう</t>
+  </si>
+  <si>
+    <t>ten</t>
+  </si>
+  <si>
+    <t>に</t>
+  </si>
+  <si>
+    <t>two</t>
+  </si>
+  <si>
+    <t>ほん</t>
+  </si>
+  <si>
+    <t>book; origin</t>
+  </si>
+  <si>
+    <t>なか</t>
+  </si>
+  <si>
+    <t>inside; middle</t>
+  </si>
+  <si>
+    <t>ImageName</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>日</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>day; sun</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>n5_sun.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>一</t>
-  </si>
-  <si>
-    <t>いち</t>
-  </si>
-  <si>
-    <t>one</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>n5_one.jpg</t>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>国</t>
-  </si>
-  <si>
-    <t>くに</t>
-  </si>
-  <si>
-    <t>country</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>n5_country.jpg</t>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>人</t>
-  </si>
-  <si>
-    <t>ひと</t>
-  </si>
-  <si>
-    <t>person</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>n5_person.webp</t>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>年</t>
-  </si>
-  <si>
-    <t>とし</t>
-  </si>
-  <si>
-    <t>year</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>n5_year.jpg</t>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>大</t>
-  </si>
-  <si>
-    <t>おおきい</t>
-  </si>
-  <si>
-    <t>big</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>n5_big.webp</t>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>十</t>
-  </si>
-  <si>
-    <t>じゅう</t>
-  </si>
-  <si>
-    <t>ten</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>n5_ten.jpg</t>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>二</t>
-  </si>
-  <si>
-    <t>に</t>
-  </si>
-  <si>
-    <t>two</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>n5_two.png</t>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>本</t>
-  </si>
-  <si>
-    <t>ほん</t>
-  </si>
-  <si>
-    <t>book; origin</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>n5_book.png</t>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>中</t>
-  </si>
-  <si>
-    <t>なか</t>
-  </si>
-  <si>
-    <t>inside; middle</t>
-  </si>
-  <si>
-    <t>ImageName</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>日</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>day; sun</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>n5_sun.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>n5_inside.webp</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -170,8 +215,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -477,7 +525,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -499,120 +547,147 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
+      <c r="D3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
+      <c r="D4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>17</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>21</v>
+      </c>
+      <c r="D11" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>